<commit_message>
Search User Using Name
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="44">
   <si>
     <t/>
   </si>
@@ -120,6 +120,30 @@
   </si>
   <si>
     <t>AddUser_ToastMessage</t>
+  </si>
+  <si>
+    <t>SearchUser_SearchByDropdown</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div[1]/div/div[2]/div/div[2]/div/div[2]/div[1]/div[1]/div[1]/select</t>
+  </si>
+  <si>
+    <t>SearchUser_SearchBar</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Search...']</t>
+  </si>
+  <si>
+    <t>SearchUser_SearchButton</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div[1]/div/div[2]/div/div[2]/div/div[2]/div[1]/div[1]/div[2]/button</t>
+  </si>
+  <si>
+    <t>SearchUser_Result</t>
+  </si>
+  <si>
+    <t>//td[normalize-space()='Kasun Bandara']</t>
   </si>
 </sst>
 </file>
@@ -164,7 +188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -368,6 +392,83 @@
         <v>6</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Search User Using Role
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="46">
   <si>
     <t/>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>//td[normalize-space()='Kasun Bandara']</t>
+  </si>
+  <si>
+    <t>SearchUser_Result2</t>
+  </si>
+  <si>
+    <t>//td[normalize-space()='Admin']</t>
   </si>
 </sst>
 </file>
@@ -449,13 +455,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">

</xml_diff>

<commit_message>
Search User Using Email
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t/>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>//td[normalize-space()='Admin']</t>
+  </si>
+  <si>
+    <t>SearchUser_Result3</t>
+  </si>
+  <si>
+    <t>//td[normalize-space()='kasun@gmail.com']</t>
   </si>
 </sst>
 </file>
@@ -466,13 +472,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search User Using Address
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="50">
   <si>
     <t/>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>//td[normalize-space()='kasun@gmail.com']</t>
+  </si>
+  <si>
+    <t>SearchUser_Result4</t>
+  </si>
+  <si>
+    <t>//td[normalize-space()='Dewalegama,Kegalle']</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -481,6 +487,61 @@
         <v>6</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Change User Password Functionality
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="63">
   <si>
     <t/>
   </si>
@@ -174,6 +174,33 @@
   </si>
   <si>
     <t>//button[normalize-space()='Update']</t>
+  </si>
+  <si>
+    <t>EditUser_ToastMessage</t>
+  </si>
+  <si>
+    <t>UserChangePassword_Action</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div[1]/div/div[2]/div/div[2]/div/div[3]/div/table/tbody/tr[3]/td[6]/div/button[2]</t>
+  </si>
+  <si>
+    <t>User_NewPassword</t>
+  </si>
+  <si>
+    <t>User_ConfirmPassword</t>
+  </si>
+  <si>
+    <t>(//input[@placeholder='xxxxxxxx'])[2]</t>
+  </si>
+  <si>
+    <t>User_PasswordResetButton</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='Reset']</t>
+  </si>
+  <si>
+    <t>ChangePassword_ToastMessage</t>
   </si>
 </sst>
 </file>
@@ -218,7 +245,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -512,21 +539,21 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>6</v>
@@ -534,23 +561,133 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C30" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
User Page Size Functionality
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="65">
   <si>
     <t/>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>ChangePassword_ToastMessage</t>
+  </si>
+  <si>
+    <t>UserPageSizeDropdown</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='10']</t>
   </si>
 </sst>
 </file>
@@ -660,13 +666,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39">

</xml_diff>